<commit_message>
feat: added formula evaluator
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -8,8 +8,8 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mge7zQ7GA6pqOwk5aC7btxfphbB/Q=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="31TbsXSoahfDFGtgNQeLRULbkl1I0piGUexVKPFHETs="/>
     </ext>
   </extLst>
 </workbook>
@@ -79,7 +79,7 @@
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="yyyy/m/d hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -94,6 +94,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Google Sans Mono&quot;"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -149,6 +154,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,8 +620,11 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="11">
+        <f>SUM(H2:H6)</f>
+        <v>47778</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>

</xml_diff>